<commit_message>
made a script to initialize dummy data with datadictionary
</commit_message>
<xml_diff>
--- a/initData/datadictionary.xlsx
+++ b/initData/datadictionary.xlsx
@@ -2137,23 +2137,37 @@
       <c r="A42" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="B42" s="27"/>
-      <c r="C42" s="27"/>
-      <c r="D42" s="27"/>
-      <c r="E42" s="27"/>
-      <c r="F42" s="27"/>
-      <c r="G42" s="27"/>
-      <c r="H42" s="27"/>
-      <c r="I42" s="27"/>
+      <c r="B42" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C42" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="D42" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E42" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="F42" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="G42" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="H42" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="I42" s="28"/>
       <c r="J42" s="28"/>
     </row>
     <row r="43">
-      <c r="A43" s="27"/>
+      <c r="A43" s="28"/>
       <c r="B43" s="27" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C43" s="27" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="D43" s="27" t="s">
         <v>20</v>
@@ -2167,28 +2181,26 @@
       <c r="G43" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="H43" s="27" t="s">
-        <v>78</v>
-      </c>
+      <c r="H43" s="28"/>
       <c r="I43" s="28"/>
       <c r="J43" s="28"/>
     </row>
     <row r="44">
       <c r="A44" s="28"/>
       <c r="B44" s="27" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D44" s="27" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="E44" s="27" t="s">
-        <v>114</v>
+        <v>40</v>
       </c>
       <c r="F44" s="27" t="s">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="G44" s="27" t="s">
         <v>16</v>
@@ -2198,824 +2210,752 @@
       <c r="J44" s="28"/>
     </row>
     <row r="45">
-      <c r="A45" s="28"/>
-      <c r="B45" s="27" t="s">
+      <c r="A45" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="B45" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="C45" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="D45" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="E45" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="F45" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="G45" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="H45" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="29"/>
+      <c r="B46" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="C46" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="D46" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="E46" s="31">
+        <v>4.294967295E9</v>
+      </c>
+      <c r="F46" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="G46" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="H46" s="30"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="29" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="30"/>
+      <c r="B47" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="C45" s="27" t="s">
+      <c r="C47" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="D45" s="27" t="s">
+      <c r="D47" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="E45" s="27" t="s">
+      <c r="E47" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="F45" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="G45" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="H45" s="28"/>
-      <c r="I45" s="28"/>
-      <c r="J45" s="28"/>
-    </row>
-    <row r="46">
-      <c r="A46" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="B46" s="29"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="29"/>
-      <c r="E46" s="29"/>
-      <c r="F46" s="29"/>
-      <c r="G46" s="29"/>
-      <c r="H46" s="29"/>
-      <c r="I46" s="29"/>
-      <c r="J46" s="30"/>
-    </row>
-    <row r="47">
-      <c r="A47" s="29"/>
-      <c r="B47" s="29" t="s">
+      <c r="F47" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="G47" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="H47" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="I47" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="J47" s="29" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="B48" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="C47" s="29" t="s">
+      <c r="C48" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="D47" s="29" t="s">
+      <c r="D48" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="E47" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="F47" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="G47" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="H47" s="29" t="s">
+      <c r="E48" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="F48" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="G48" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="H48" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="I47" s="30"/>
-      <c r="J47" s="30"/>
-    </row>
-    <row r="48">
-      <c r="A48" s="30"/>
-      <c r="B48" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="C48" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="D48" s="29" t="s">
+      <c r="I48" s="33"/>
+      <c r="J48" s="32"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="33"/>
+      <c r="B49" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C49" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="D49" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="E49" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="F49" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="G49" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="H49" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="I49" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="J49" s="32" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="33"/>
+      <c r="B50" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="C50" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="D50" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="E50" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="F50" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="G50" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="H50" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="I50" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="J50" s="33"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="33"/>
+      <c r="B51" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="C51" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="D51" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="E48" s="31">
+      <c r="E51" s="34">
         <v>4.294967295E9</v>
       </c>
-      <c r="F48" s="29" t="s">
+      <c r="F51" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="G48" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="H48" s="30"/>
-      <c r="I48" s="30"/>
-      <c r="J48" s="29" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="30"/>
-      <c r="B49" s="29" t="s">
+      <c r="G51" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="H51" s="33"/>
+      <c r="I51" s="33"/>
+      <c r="J51" s="33"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="B52" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="C52" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="D52" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="E52" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="F52" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="G52" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="H52" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="I52" s="36"/>
+      <c r="J52" s="35"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="36"/>
+      <c r="B53" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="C53" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="D53" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="E53" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="F53" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G53" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="H53" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="I53" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="J53" s="36"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="36"/>
+      <c r="B54" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="C54" s="35" t="s">
+        <v>139</v>
+      </c>
+      <c r="D54" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="E54" s="35" t="s">
+        <v>141</v>
+      </c>
+      <c r="F54" s="38" t="s">
+        <v>142</v>
+      </c>
+      <c r="G54" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="H54" s="36"/>
+      <c r="I54" s="36"/>
+      <c r="J54" s="35" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="36"/>
+      <c r="B55" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="C49" s="29" t="s">
+      <c r="C55" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="D49" s="29" t="s">
+      <c r="D55" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="E49" s="29" t="s">
+      <c r="E55" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="F49" s="29" t="s">
+      <c r="F55" s="35" t="s">
         <v>129</v>
       </c>
-      <c r="G49" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="H49" s="29" t="s">
+      <c r="G55" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="H55" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="I49" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="J49" s="29" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="32" t="s">
-        <v>131</v>
-      </c>
-      <c r="B50" s="32"/>
-      <c r="C50" s="32"/>
-      <c r="D50" s="32"/>
-      <c r="E50" s="32"/>
-      <c r="F50" s="32"/>
-      <c r="G50" s="32"/>
-      <c r="H50" s="33"/>
-      <c r="I50" s="33"/>
-      <c r="J50" s="32"/>
-    </row>
-    <row r="51">
-      <c r="A51" s="32"/>
-      <c r="B51" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="C51" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="D51" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="E51" s="32" t="s">
-        <v>132</v>
-      </c>
-      <c r="F51" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="G51" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="H51" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="I51" s="33"/>
-      <c r="J51" s="32"/>
-    </row>
-    <row r="52">
-      <c r="A52" s="33"/>
-      <c r="B52" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="C52" s="32" t="s">
-        <v>122</v>
-      </c>
-      <c r="D52" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="E52" s="32" t="s">
-        <v>132</v>
-      </c>
-      <c r="F52" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="G52" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="H52" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="I52" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="J52" s="32" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="33"/>
-      <c r="B53" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="C53" s="32" t="s">
-        <v>123</v>
-      </c>
-      <c r="D53" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="E53" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="F53" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="G53" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="H53" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="I53" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="J53" s="33"/>
-    </row>
-    <row r="54">
-      <c r="A54" s="33"/>
-      <c r="B54" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="C54" s="32" t="s">
-        <v>136</v>
-      </c>
-      <c r="D54" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="E54" s="34">
-        <v>4.294967295E9</v>
-      </c>
-      <c r="F54" s="34" t="s">
-        <v>127</v>
-      </c>
-      <c r="G54" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="H54" s="33"/>
-      <c r="I54" s="33"/>
-      <c r="J54" s="33"/>
-    </row>
-    <row r="55">
-      <c r="A55" s="35" t="s">
-        <v>137</v>
-      </c>
-      <c r="B55" s="35"/>
-      <c r="C55" s="35"/>
-      <c r="D55" s="35"/>
-      <c r="E55" s="35"/>
-      <c r="F55" s="35"/>
-      <c r="G55" s="35"/>
-      <c r="H55" s="36"/>
       <c r="I55" s="36"/>
       <c r="J55" s="36"/>
     </row>
     <row r="56">
-      <c r="A56" s="35"/>
-      <c r="B56" s="35" t="s">
+      <c r="A56" s="39" t="s">
+        <v>144</v>
+      </c>
+      <c r="B56" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="C56" s="35" t="s">
+      <c r="C56" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="D56" s="35" t="s">
+      <c r="D56" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="E56" s="35" t="s">
+      <c r="E56" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="F56" s="35" t="s">
+      <c r="F56" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="G56" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="H56" s="35" t="s">
+      <c r="G56" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="H56" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="I56" s="36"/>
-      <c r="J56" s="35"/>
+      <c r="I56" s="40"/>
+      <c r="J56" s="40"/>
     </row>
     <row r="57">
-      <c r="A57" s="36"/>
-      <c r="B57" s="35" t="s">
+      <c r="A57" s="39"/>
+      <c r="B57" s="39" t="s">
+        <v>145</v>
+      </c>
+      <c r="C57" s="39" t="s">
+        <v>146</v>
+      </c>
+      <c r="D57" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="E57" s="41">
+        <v>4.294967295E9</v>
+      </c>
+      <c r="F57" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="G57" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="H57" s="40"/>
+      <c r="I57" s="40"/>
+      <c r="J57" s="39"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="40"/>
+      <c r="B58" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="C58" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="D58" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="E58" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="F58" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="G58" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="H58" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="I58" s="40"/>
+      <c r="J58" s="40"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="B59" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="C57" s="35" t="s">
+      <c r="C59" s="42" t="s">
         <v>138</v>
       </c>
-      <c r="D57" s="35" t="s">
+      <c r="D59" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="E57" s="35" t="s">
+      <c r="E59" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="F57" s="37" t="s">
+      <c r="F59" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="G57" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="H57" s="35" t="s">
+      <c r="G59" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="H59" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="I57" s="35" t="s">
+      <c r="I59" s="42" t="s">
         <v>133</v>
       </c>
-      <c r="J57" s="36"/>
-    </row>
-    <row r="58">
-      <c r="A58" s="36"/>
-      <c r="B58" s="35" t="s">
-        <v>135</v>
-      </c>
-      <c r="C58" s="35" t="s">
-        <v>139</v>
-      </c>
-      <c r="D58" s="35" t="s">
-        <v>140</v>
-      </c>
-      <c r="E58" s="35" t="s">
-        <v>141</v>
-      </c>
-      <c r="F58" s="38" t="s">
-        <v>142</v>
-      </c>
-      <c r="G58" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="H58" s="36"/>
-      <c r="I58" s="36"/>
-      <c r="J58" s="35" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="36"/>
-      <c r="B59" s="35" t="s">
+      <c r="J59" s="44"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="42"/>
+      <c r="B60" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="C60" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="D60" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="E60" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="F60" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="G60" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="H60" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="I60" s="44"/>
+      <c r="J60" s="42"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="44"/>
+      <c r="B61" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="C59" s="35" t="s">
+      <c r="C61" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="D59" s="35" t="s">
+      <c r="D61" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="E59" s="35" t="s">
+      <c r="E61" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="F59" s="35" t="s">
+      <c r="F61" s="42" t="s">
         <v>129</v>
       </c>
-      <c r="G59" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="H59" s="35" t="s">
+      <c r="G61" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="H61" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="I59" s="36"/>
-      <c r="J59" s="36"/>
-    </row>
-    <row r="60">
-      <c r="A60" s="39" t="s">
-        <v>144</v>
-      </c>
-      <c r="B60" s="39"/>
-      <c r="C60" s="39"/>
-      <c r="D60" s="39"/>
-      <c r="E60" s="39"/>
-      <c r="F60" s="39"/>
-      <c r="G60" s="39"/>
-      <c r="H60" s="40"/>
-      <c r="I60" s="40"/>
-      <c r="J60" s="40"/>
-    </row>
-    <row r="61">
-      <c r="A61" s="39"/>
-      <c r="B61" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="C61" s="39" t="s">
-        <v>107</v>
-      </c>
-      <c r="D61" s="39" t="s">
+      <c r="I61" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="J61" s="44"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="45" t="s">
+        <v>147</v>
+      </c>
+      <c r="B62" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="C62" s="45" t="s">
+        <v>148</v>
+      </c>
+      <c r="D62" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="E61" s="39" t="s">
-        <v>132</v>
-      </c>
-      <c r="F61" s="39" t="s">
+      <c r="E62" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="F62" s="45" t="s">
+        <v>149</v>
+      </c>
+      <c r="G62" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="H62" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="I62" s="46"/>
+      <c r="J62" s="46"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="46"/>
+      <c r="B63" s="45" t="s">
+        <v>150</v>
+      </c>
+      <c r="C63" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="D63" s="45" t="s">
+        <v>152</v>
+      </c>
+      <c r="E63" s="45" t="s">
+        <v>153</v>
+      </c>
+      <c r="F63" s="46"/>
+      <c r="G63" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="H63" s="46"/>
+      <c r="I63" s="46"/>
+      <c r="J63" s="46"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="46"/>
+      <c r="B64" s="45" t="s">
+        <v>154</v>
+      </c>
+      <c r="C64" s="45" t="s">
+        <v>155</v>
+      </c>
+      <c r="D64" s="45" t="s">
+        <v>156</v>
+      </c>
+      <c r="E64" s="45">
+        <v>1.6777215E7</v>
+      </c>
+      <c r="F64" s="45" t="s">
+        <v>157</v>
+      </c>
+      <c r="G64" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="H64" s="46"/>
+      <c r="I64" s="46"/>
+      <c r="J64" s="46"/>
+    </row>
+    <row r="65">
+      <c r="A65" s="46"/>
+      <c r="B65" s="45" t="s">
+        <v>131</v>
+      </c>
+      <c r="C65" s="45" t="s">
+        <v>158</v>
+      </c>
+      <c r="D65" s="45" t="s">
+        <v>159</v>
+      </c>
+      <c r="E65" s="45">
+        <v>9.999</v>
+      </c>
+      <c r="F65" s="45" t="s">
+        <v>160</v>
+      </c>
+      <c r="G65" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="H65" s="46"/>
+      <c r="I65" s="46"/>
+      <c r="J65" s="45" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="46"/>
+      <c r="B66" s="45" t="s">
+        <v>162</v>
+      </c>
+      <c r="C66" s="45" t="s">
+        <v>163</v>
+      </c>
+      <c r="D66" s="45" t="s">
+        <v>164</v>
+      </c>
+      <c r="E66" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="F66" s="45" t="s">
+        <v>149</v>
+      </c>
+      <c r="G66" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="H66" s="46"/>
+      <c r="I66" s="46"/>
+      <c r="J66" s="46"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="46"/>
+      <c r="B67" s="45" t="s">
+        <v>165</v>
+      </c>
+      <c r="C67" s="45" t="s">
+        <v>166</v>
+      </c>
+      <c r="D67" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="E67" s="47">
+        <v>4.294967295E9</v>
+      </c>
+      <c r="F67" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="G67" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="H67" s="46"/>
+      <c r="I67" s="46"/>
+      <c r="J67" s="45" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="B68" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="C68" s="48" t="s">
+        <v>138</v>
+      </c>
+      <c r="D68" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="E68" s="48" t="s">
+        <v>169</v>
+      </c>
+      <c r="F68" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="G61" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="H61" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="I61" s="40"/>
-      <c r="J61" s="39"/>
-    </row>
-    <row r="62">
-      <c r="A62" s="40"/>
-      <c r="B62" s="39" t="s">
-        <v>145</v>
-      </c>
-      <c r="C62" s="39" t="s">
-        <v>146</v>
-      </c>
-      <c r="D62" s="39" t="s">
-        <v>84</v>
-      </c>
-      <c r="E62" s="41">
-        <v>4.294967295E9</v>
-      </c>
-      <c r="F62" s="41" t="s">
-        <v>85</v>
-      </c>
-      <c r="G62" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="H62" s="40"/>
-      <c r="I62" s="40"/>
-      <c r="J62" s="40"/>
-    </row>
-    <row r="63">
-      <c r="A63" s="40"/>
-      <c r="B63" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="C63" s="39" t="s">
-        <v>123</v>
-      </c>
-      <c r="D63" s="39" t="s">
+      <c r="G68" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="H68" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="I68" s="48" t="s">
+        <v>133</v>
+      </c>
+      <c r="J68" s="50"/>
+    </row>
+    <row r="69">
+      <c r="A69" s="50"/>
+      <c r="B69" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="C69" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="D69" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="E63" s="39" t="s">
+      <c r="E69" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="F63" s="39" t="s">
+      <c r="F69" s="48" t="s">
         <v>129</v>
       </c>
-      <c r="G63" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="H63" s="39" t="s">
-        <v>46</v>
-      </c>
-      <c r="I63" s="40"/>
-      <c r="J63" s="40"/>
-    </row>
-    <row r="64">
-      <c r="A64" s="42" t="s">
-        <v>133</v>
-      </c>
-      <c r="B64" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="C64" s="42" t="s">
-        <v>138</v>
-      </c>
-      <c r="D64" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="E64" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="F64" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="G64" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="H64" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="I64" s="42" t="s">
-        <v>133</v>
-      </c>
-      <c r="J64" s="44"/>
-    </row>
-    <row r="65">
-      <c r="A65" s="42"/>
-      <c r="B65" s="42" t="s">
-        <v>54</v>
-      </c>
-      <c r="C65" s="42" t="s">
-        <v>107</v>
-      </c>
-      <c r="D65" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="E65" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="F65" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="G65" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="H65" s="42" t="s">
+      <c r="G69" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="H69" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="I69" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="J69" s="50"/>
+    </row>
+    <row r="70">
+      <c r="A70" s="51" t="s">
+        <v>172</v>
+      </c>
+      <c r="B70" s="51" t="s">
+        <v>170</v>
+      </c>
+      <c r="C70" s="51" t="s">
+        <v>173</v>
+      </c>
+      <c r="D70" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="E70" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="F70" s="51" t="s">
+        <v>129</v>
+      </c>
+      <c r="G70" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="H70" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="I65" s="44"/>
-      <c r="J65" s="42"/>
-    </row>
-    <row r="66">
-      <c r="A66" s="44"/>
-      <c r="B66" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="C66" s="42" t="s">
-        <v>123</v>
-      </c>
-      <c r="D66" s="42" t="s">
-        <v>39</v>
-      </c>
-      <c r="E66" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="F66" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="G66" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="H66" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="I66" s="42" t="s">
-        <v>43</v>
-      </c>
-      <c r="J66" s="44"/>
-    </row>
-    <row r="67">
-      <c r="A67" s="45" t="s">
-        <v>147</v>
-      </c>
-      <c r="B67" s="45" t="s">
-        <v>50</v>
-      </c>
-      <c r="C67" s="45" t="s">
-        <v>148</v>
-      </c>
-      <c r="D67" s="45" t="s">
-        <v>20</v>
-      </c>
-      <c r="E67" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="F67" s="45" t="s">
-        <v>149</v>
-      </c>
-      <c r="G67" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="H67" s="45" t="s">
-        <v>78</v>
-      </c>
-      <c r="I67" s="46"/>
-      <c r="J67" s="46"/>
-    </row>
-    <row r="68">
-      <c r="A68" s="46"/>
-      <c r="B68" s="45" t="s">
-        <v>150</v>
-      </c>
-      <c r="C68" s="45" t="s">
-        <v>151</v>
-      </c>
-      <c r="D68" s="45" t="s">
-        <v>152</v>
-      </c>
-      <c r="E68" s="45" t="s">
-        <v>153</v>
-      </c>
-      <c r="F68" s="46"/>
-      <c r="G68" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="H68" s="46"/>
-      <c r="I68" s="46"/>
-      <c r="J68" s="46"/>
-    </row>
-    <row r="69">
-      <c r="A69" s="46"/>
-      <c r="B69" s="45" t="s">
-        <v>154</v>
-      </c>
-      <c r="C69" s="45" t="s">
-        <v>155</v>
-      </c>
-      <c r="D69" s="45" t="s">
-        <v>156</v>
-      </c>
-      <c r="E69" s="45">
-        <v>1.6777215E7</v>
-      </c>
-      <c r="F69" s="45" t="s">
-        <v>157</v>
-      </c>
-      <c r="G69" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="H69" s="46"/>
-      <c r="I69" s="46"/>
-      <c r="J69" s="46"/>
-    </row>
-    <row r="70">
-      <c r="A70" s="46"/>
-      <c r="B70" s="45" t="s">
-        <v>131</v>
-      </c>
-      <c r="C70" s="45" t="s">
-        <v>158</v>
-      </c>
-      <c r="D70" s="45" t="s">
+      <c r="I70" s="52"/>
+      <c r="J70" s="52"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="52"/>
+      <c r="B71" s="51" t="s">
+        <v>174</v>
+      </c>
+      <c r="C71" s="51" t="s">
+        <v>175</v>
+      </c>
+      <c r="D71" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="E71" s="51" t="s">
+        <v>169</v>
+      </c>
+      <c r="F71" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="G71" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="H71" s="52"/>
+      <c r="I71" s="52"/>
+      <c r="J71" s="52"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="52"/>
+      <c r="B72" s="51" t="s">
+        <v>176</v>
+      </c>
+      <c r="C72" s="51" t="s">
+        <v>177</v>
+      </c>
+      <c r="D72" s="51" t="s">
         <v>159</v>
       </c>
-      <c r="E70" s="45">
+      <c r="E72" s="51">
         <v>9.999</v>
       </c>
-      <c r="F70" s="45" t="s">
+      <c r="F72" s="51" t="s">
         <v>160</v>
       </c>
-      <c r="G70" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="H70" s="46"/>
-      <c r="I70" s="46"/>
-      <c r="J70" s="45" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" s="46"/>
-      <c r="B71" s="45" t="s">
-        <v>162</v>
-      </c>
-      <c r="C71" s="45" t="s">
-        <v>163</v>
-      </c>
-      <c r="D71" s="45" t="s">
-        <v>164</v>
-      </c>
-      <c r="E71" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="F71" s="45" t="s">
-        <v>149</v>
-      </c>
-      <c r="G71" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="H71" s="46"/>
-      <c r="I71" s="46"/>
-      <c r="J71" s="46"/>
-    </row>
-    <row r="72">
-      <c r="A72" s="46"/>
-      <c r="B72" s="45" t="s">
-        <v>165</v>
-      </c>
-      <c r="C72" s="45" t="s">
-        <v>166</v>
-      </c>
-      <c r="D72" s="45" t="s">
-        <v>84</v>
-      </c>
-      <c r="E72" s="47">
-        <v>4.294967295E9</v>
-      </c>
-      <c r="F72" s="47" t="s">
-        <v>85</v>
-      </c>
-      <c r="G72" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="H72" s="46"/>
-      <c r="I72" s="46"/>
-      <c r="J72" s="45" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" s="48" t="s">
-        <v>168</v>
-      </c>
-      <c r="B73" s="48" t="s">
-        <v>50</v>
-      </c>
-      <c r="C73" s="48" t="s">
-        <v>138</v>
-      </c>
-      <c r="D73" s="48" t="s">
-        <v>20</v>
-      </c>
-      <c r="E73" s="48" t="s">
-        <v>169</v>
-      </c>
-      <c r="F73" s="49" t="s">
-        <v>22</v>
-      </c>
-      <c r="G73" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="H73" s="48" t="s">
-        <v>66</v>
-      </c>
-      <c r="I73" s="48" t="s">
-        <v>133</v>
-      </c>
-      <c r="J73" s="50"/>
-    </row>
-    <row r="74">
-      <c r="A74" s="50"/>
-      <c r="B74" s="48" t="s">
-        <v>170</v>
-      </c>
-      <c r="C74" s="48" t="s">
-        <v>171</v>
-      </c>
-      <c r="D74" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="E74" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="F74" s="48" t="s">
-        <v>129</v>
-      </c>
-      <c r="G74" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="H74" s="48" t="s">
-        <v>66</v>
-      </c>
-      <c r="I74" s="48" t="s">
-        <v>172</v>
-      </c>
-      <c r="J74" s="50"/>
-    </row>
-    <row r="75">
-      <c r="A75" s="51" t="s">
-        <v>172</v>
-      </c>
-      <c r="B75" s="51" t="s">
-        <v>170</v>
-      </c>
-      <c r="C75" s="51" t="s">
-        <v>173</v>
-      </c>
-      <c r="D75" s="51" t="s">
-        <v>39</v>
-      </c>
-      <c r="E75" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="F75" s="51" t="s">
-        <v>129</v>
-      </c>
-      <c r="G75" s="51" t="s">
-        <v>16</v>
-      </c>
-      <c r="H75" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="I75" s="52"/>
-      <c r="J75" s="52"/>
-    </row>
-    <row r="76">
-      <c r="A76" s="52"/>
-      <c r="B76" s="51" t="s">
-        <v>174</v>
-      </c>
-      <c r="C76" s="51" t="s">
-        <v>175</v>
-      </c>
-      <c r="D76" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="E76" s="51" t="s">
-        <v>169</v>
-      </c>
-      <c r="F76" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="G76" s="51" t="s">
-        <v>16</v>
-      </c>
-      <c r="H76" s="52"/>
-      <c r="I76" s="52"/>
-      <c r="J76" s="52"/>
-    </row>
-    <row r="77">
-      <c r="A77" s="52"/>
-      <c r="B77" s="51" t="s">
-        <v>176</v>
-      </c>
-      <c r="C77" s="51" t="s">
-        <v>177</v>
-      </c>
-      <c r="D77" s="51" t="s">
-        <v>159</v>
-      </c>
-      <c r="E77" s="51">
-        <v>9.999</v>
-      </c>
-      <c r="F77" s="51" t="s">
-        <v>160</v>
-      </c>
-      <c r="G77" s="51" t="s">
-        <v>16</v>
-      </c>
-      <c r="H77" s="52"/>
-      <c r="I77" s="52"/>
-      <c r="J77" s="52"/>
+      <c r="G72" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="H72" s="52"/>
+      <c r="I72" s="52"/>
+      <c r="J72" s="52"/>
     </row>
   </sheetData>
   <printOptions gridLines="1" horizontalCentered="1"/>

</xml_diff>